<commit_message>
Practice : BST Deletion has issues!
</commit_message>
<xml_diff>
--- a/Documents/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/Documents/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="510" windowWidth="22710" windowHeight="8940"/>
+    <workbookView xWindow="216" yWindow="516" windowWidth="22716" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="DSA in 2.5 Months" sheetId="1" r:id="rId1"/>
@@ -16,14 +16,14 @@
   </definedNames>
   <calcPr calcId="124519"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{C1A4E709-E9F1-4376-A047-F26FFC5F2C8F}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{5451177E-605B-4368-AC7B-D46C41798C55}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{C1A4E709-E9F1-4376-A047-F26FFC5F2C8F}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="469">
   <si>
     <t>DSA by Shradha Didi &amp; Aman Bhaiya</t>
   </si>
@@ -1443,6 +1443,9 @@
   </si>
   <si>
     <t>Solved</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -1682,7 +1685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1812,6 +1815,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2026,17 +2030,17 @@
   </sheetPr>
   <dimension ref="A1:Z919"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="E250" sqref="E250"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="88.28515625" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="88.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="32.25" customHeight="1">
@@ -4628,7 +4632,7 @@
       <c r="Y80" s="2"/>
       <c r="Z80" s="2"/>
     </row>
-    <row r="81" spans="1:26">
+    <row r="81" spans="1:26" ht="15.6">
       <c r="A81" s="24" t="s">
         <v>99</v>
       </c>
@@ -4660,7 +4664,7 @@
       <c r="Y81" s="2"/>
       <c r="Z81" s="2"/>
     </row>
-    <row r="82" spans="1:26">
+    <row r="82" spans="1:26" ht="15.6">
       <c r="A82" s="26" t="s">
         <v>99</v>
       </c>
@@ -4692,7 +4696,7 @@
       <c r="Y82" s="2"/>
       <c r="Z82" s="2"/>
     </row>
-    <row r="83" spans="1:26">
+    <row r="83" spans="1:26" ht="15.6">
       <c r="A83" s="26" t="s">
         <v>99</v>
       </c>
@@ -4724,7 +4728,7 @@
       <c r="Y83" s="2"/>
       <c r="Z83" s="2"/>
     </row>
-    <row r="84" spans="1:26">
+    <row r="84" spans="1:26" ht="15.6">
       <c r="A84" s="26" t="s">
         <v>99</v>
       </c>
@@ -4755,7 +4759,7 @@
       <c r="Y84" s="2"/>
       <c r="Z84" s="2"/>
     </row>
-    <row r="85" spans="1:26">
+    <row r="85" spans="1:26" ht="15.6">
       <c r="A85" s="26" t="s">
         <v>99</v>
       </c>
@@ -4786,7 +4790,7 @@
       <c r="Y85" s="2"/>
       <c r="Z85" s="2"/>
     </row>
-    <row r="86" spans="1:26">
+    <row r="86" spans="1:26" ht="15.6">
       <c r="A86" s="26" t="s">
         <v>99</v>
       </c>
@@ -4818,7 +4822,7 @@
       <c r="Y86" s="2"/>
       <c r="Z86" s="2"/>
     </row>
-    <row r="87" spans="1:26">
+    <row r="87" spans="1:26" ht="15.6">
       <c r="A87" s="26" t="s">
         <v>99</v>
       </c>
@@ -4850,7 +4854,7 @@
       <c r="Y87" s="2"/>
       <c r="Z87" s="2"/>
     </row>
-    <row r="88" spans="1:26">
+    <row r="88" spans="1:26" ht="15.6">
       <c r="A88" s="26" t="s">
         <v>99</v>
       </c>
@@ -4882,7 +4886,7 @@
       <c r="Y88" s="2"/>
       <c r="Z88" s="2"/>
     </row>
-    <row r="89" spans="1:26">
+    <row r="89" spans="1:26" ht="15.6">
       <c r="A89" s="26" t="s">
         <v>99</v>
       </c>
@@ -4914,7 +4918,7 @@
       <c r="Y89" s="2"/>
       <c r="Z89" s="2"/>
     </row>
-    <row r="90" spans="1:26">
+    <row r="90" spans="1:26" ht="15.6">
       <c r="A90" s="26" t="s">
         <v>99</v>
       </c>
@@ -4946,7 +4950,7 @@
       <c r="Y90" s="2"/>
       <c r="Z90" s="2"/>
     </row>
-    <row r="91" spans="1:26">
+    <row r="91" spans="1:26" ht="15.6">
       <c r="A91" s="26" t="s">
         <v>99</v>
       </c>
@@ -4978,7 +4982,7 @@
       <c r="Y91" s="2"/>
       <c r="Z91" s="2"/>
     </row>
-    <row r="92" spans="1:26">
+    <row r="92" spans="1:26" ht="15.6">
       <c r="A92" s="28" t="s">
         <v>99</v>
       </c>
@@ -5010,7 +5014,7 @@
       <c r="Y92" s="2"/>
       <c r="Z92" s="2"/>
     </row>
-    <row r="93" spans="1:26">
+    <row r="93" spans="1:26" ht="15.6">
       <c r="A93" s="28" t="s">
         <v>99</v>
       </c>
@@ -5042,7 +5046,7 @@
       <c r="Y93" s="2"/>
       <c r="Z93" s="2"/>
     </row>
-    <row r="94" spans="1:26">
+    <row r="94" spans="1:26" ht="15.6">
       <c r="A94" s="28" t="s">
         <v>99</v>
       </c>
@@ -5074,7 +5078,7 @@
       <c r="Y94" s="2"/>
       <c r="Z94" s="2"/>
     </row>
-    <row r="95" spans="1:26">
+    <row r="95" spans="1:26" ht="15.6">
       <c r="A95" s="28" t="s">
         <v>99</v>
       </c>
@@ -5106,7 +5110,7 @@
       <c r="Y95" s="2"/>
       <c r="Z95" s="2"/>
     </row>
-    <row r="96" spans="1:26">
+    <row r="96" spans="1:26" ht="15.6">
       <c r="A96" s="28" t="s">
         <v>99</v>
       </c>
@@ -5138,7 +5142,7 @@
       <c r="Y96" s="2"/>
       <c r="Z96" s="2"/>
     </row>
-    <row r="97" spans="1:26">
+    <row r="97" spans="1:26" ht="15.6">
       <c r="A97" s="28" t="s">
         <v>99</v>
       </c>
@@ -5170,7 +5174,7 @@
       <c r="Y97" s="2"/>
       <c r="Z97" s="2"/>
     </row>
-    <row r="98" spans="1:26">
+    <row r="98" spans="1:26" ht="15.6">
       <c r="A98" s="28" t="s">
         <v>99</v>
       </c>
@@ -9838,6 +9842,9 @@
         <v>268</v>
       </c>
       <c r="C249" s="20"/>
+      <c r="E249" s="45" t="s">
+        <v>468</v>
+      </c>
       <c r="F249" s="2"/>
       <c r="G249" s="2"/>
       <c r="H249" s="2"/>
@@ -11201,7 +11208,9 @@
       </c>
       <c r="C293" s="20"/>
       <c r="D293" s="33"/>
-      <c r="E293" s="2"/>
+      <c r="E293" s="39" t="s">
+        <v>468</v>
+      </c>
       <c r="F293" s="2"/>
       <c r="G293" s="2"/>
       <c r="H293" s="2"/>
@@ -11233,7 +11242,9 @@
       </c>
       <c r="C294" s="20"/>
       <c r="D294" s="33"/>
-      <c r="E294" s="2"/>
+      <c r="E294" s="39" t="s">
+        <v>468</v>
+      </c>
       <c r="F294" s="2"/>
       <c r="G294" s="2"/>
       <c r="H294" s="2"/>
@@ -11521,7 +11532,9 @@
       </c>
       <c r="C303" s="20"/>
       <c r="D303" s="33"/>
-      <c r="E303" s="2"/>
+      <c r="E303" s="39" t="s">
+        <v>468</v>
+      </c>
       <c r="F303" s="2"/>
       <c r="G303" s="2"/>
       <c r="H303" s="2"/>
@@ -11553,7 +11566,9 @@
       </c>
       <c r="C304" s="20"/>
       <c r="D304" s="33"/>
-      <c r="E304" s="2"/>
+      <c r="E304" s="39" t="s">
+        <v>468</v>
+      </c>
       <c r="F304" s="2"/>
       <c r="G304" s="2"/>
       <c r="H304" s="2"/>
@@ -29184,13 +29199,13 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{C1A4E709-E9F1-4376-A047-F26FFC5F2C8F}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:C37"/>
+    </customSheetView>
     <customSheetView guid="{5451177E-605B-4368-AC7B-D46C41798C55}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A293:C332"/>
-    </customSheetView>
-    <customSheetView guid="{C1A4E709-E9F1-4376-A047-F26FFC5F2C8F}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="3">
@@ -29591,21 +29606,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="63.42578125" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="63.44140625" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25">
+    <row r="1" spans="1:3" ht="24.6">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
     </row>
-    <row r="2" spans="1:3" ht="12.75">
+    <row r="2" spans="1:3" ht="13.2">
       <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
@@ -29681,7 +29696,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" ht="15.6">
       <c r="A15" s="26" t="s">
         <v>99</v>
       </c>
@@ -29689,7 +29704,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" ht="15.6">
       <c r="A16" s="26" t="s">
         <v>99</v>
       </c>
@@ -29697,7 +29712,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="15.6">
       <c r="A17" s="26" t="s">
         <v>99</v>
       </c>
@@ -29705,7 +29720,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="15.6">
       <c r="A18" s="26" t="s">
         <v>99</v>
       </c>
@@ -29713,7 +29728,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="15.6">
       <c r="A19" s="28" t="s">
         <v>99</v>
       </c>
@@ -29721,7 +29736,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="15.6">
       <c r="A20" s="28" t="s">
         <v>99</v>
       </c>
@@ -29729,7 +29744,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="15.6">
       <c r="A21" s="28" t="s">
         <v>99</v>
       </c>

</xml_diff>